<commit_message>
Update locale tool, add formatted attribute for Android, add how to update tool guide
</commit_message>
<xml_diff>
--- a/localization/Locale.xlsx
+++ b/localization/Locale.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tyrael/Desktop/locale/localization_managing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/OSX 2/Work/Project/core/localization/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="19940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="19940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Key</t>
   </si>
@@ -67,9 +70,6 @@
   </si>
   <si>
     <t>mobile</t>
-  </si>
-  <si>
-    <t>Your app name in English</t>
   </si>
   <si>
     <t>Your app name in French</t>
@@ -146,12 +146,27 @@
   <si>
     <t>Enter "X" in EXPORT to generate the localization</t>
   </si>
+  <si>
+    <t>Formated</t>
+  </si>
+  <si>
+    <t>Used for android only, default value and equal empty value</t>
+  </si>
+  <si>
+    <t>Used for android only, set formatted to "false"</t>
+  </si>
+  <si>
+    <t>Formatted (Android only)</t>
+  </si>
+  <si>
+    <t>Your app name in English</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -179,12 +194,6 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="25"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="16"/>
@@ -371,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -407,34 +416,31 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -442,65 +448,71 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="83">
+  <dxfs count="81">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1274,34 +1286,6 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
           <fgColor rgb="FFFF9900"/>
           <bgColor rgb="FFFF9900"/>
         </patternFill>
@@ -1938,9 +1922,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I33" sqref="I33"/>
+      <selection pane="topRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1949,24 +1933,27 @@
     <col min="2" max="2" width="28.83203125" customWidth="1"/>
     <col min="3" max="3" width="1.83203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
     <col min="6" max="6" width="8.83203125" customWidth="1"/>
     <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="9" width="24.83203125" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" customWidth="1"/>
+    <col min="9" max="9" width="35.6640625" customWidth="1"/>
     <col min="10" max="19" width="7" customWidth="1"/>
     <col min="20" max="26" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="22" t="s">
+        <v>42</v>
+      </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1997,11 +1984,11 @@
     </row>
     <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="25"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="22" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="2"/>
@@ -2029,11 +2016,11 @@
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="24"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="24"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="23"/>
       <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
@@ -2100,14 +2087,14 @@
       <c r="F5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="3"/>
@@ -2128,7 +2115,7 @@
     <row r="6" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -2137,13 +2124,13 @@
         <v>13</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="3"/>
@@ -2164,7 +2151,7 @@
     <row r="7" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="6"/>
@@ -2194,7 +2181,7 @@
     <row r="8" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -2224,7 +2211,7 @@
     <row r="9" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
@@ -2254,7 +2241,7 @@
     <row r="10" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="6"/>
@@ -2284,11 +2271,11 @@
     <row r="11" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="E11" s="10"/>
       <c r="F11" s="9" t="s">
         <v>13</v>
       </c>
@@ -2314,11 +2301,11 @@
     <row r="12" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="9" t="s">
         <v>13</v>
       </c>
@@ -2344,11 +2331,11 @@
     <row r="13" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="9" t="s">
         <v>13</v>
       </c>
@@ -2374,11 +2361,11 @@
     <row r="14" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="9" t="s">
         <v>13</v>
       </c>
@@ -2404,11 +2391,11 @@
     <row r="15" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="9" t="s">
         <v>13</v>
       </c>
@@ -2434,11 +2421,11 @@
     <row r="16" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="9" t="s">
         <v>13</v>
       </c>
@@ -28046,143 +28033,144 @@
       <c r="X1000" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="B1:B3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="82" priority="1" operator="containsText" text=" ">
+    <cfRule type="containsText" dxfId="80" priority="1" operator="containsText" text=" ">
       <formula>NOT(ISERROR(SEARCH((" "),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="81" priority="2" operator="containsText" text="]">
+    <cfRule type="containsText" dxfId="79" priority="2" operator="containsText" text="]">
       <formula>NOT(ISERROR(SEARCH(("]"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="80" priority="3" operator="containsText" text="[">
+    <cfRule type="containsText" dxfId="78" priority="3" operator="containsText" text="[">
       <formula>NOT(ISERROR(SEARCH(("["),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="79" priority="4" operator="containsText" text="}">
+    <cfRule type="containsText" dxfId="77" priority="4" operator="containsText" text="}">
       <formula>NOT(ISERROR(SEARCH(("}"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="78" priority="5" operator="containsText" text="{">
+    <cfRule type="containsText" dxfId="76" priority="5" operator="containsText" text="{">
       <formula>NOT(ISERROR(SEARCH(("{"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="77" priority="6" operator="containsText" text="&quot;">
+    <cfRule type="containsText" dxfId="75" priority="6" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH((""""),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="76" priority="7" operator="containsText" text=":">
+    <cfRule type="containsText" dxfId="74" priority="7" operator="containsText" text=":">
       <formula>NOT(ISERROR(SEARCH((":"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="75" priority="8" operator="containsText" text=";">
+    <cfRule type="containsText" dxfId="73" priority="8" operator="containsText" text=";">
       <formula>NOT(ISERROR(SEARCH((";"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="74" priority="9" operator="containsText" text="/">
+    <cfRule type="containsText" dxfId="72" priority="9" operator="containsText" text="/">
       <formula>NOT(ISERROR(SEARCH(("/"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="73" priority="10" operator="containsText" text="&gt;">
+    <cfRule type="containsText" dxfId="71" priority="10" operator="containsText" text="&gt;">
       <formula>NOT(ISERROR(SEARCH(("&gt;"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="72" priority="11" operator="containsText" text=".">
+    <cfRule type="containsText" dxfId="70" priority="11" operator="containsText" text=".">
       <formula>NOT(ISERROR(SEARCH(("."),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="71" priority="12" operator="containsText" text="&lt;">
+    <cfRule type="containsText" dxfId="69" priority="12" operator="containsText" text="&lt;">
       <formula>NOT(ISERROR(SEARCH(("&lt;"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="70" priority="13" operator="containsText" text=",">
+    <cfRule type="containsText" dxfId="68" priority="13" operator="containsText" text=",">
       <formula>NOT(ISERROR(SEARCH((","),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="69" priority="14" operator="containsText" text="\">
+    <cfRule type="containsText" dxfId="67" priority="14" operator="containsText" text="\">
       <formula>NOT(ISERROR(SEARCH(("\"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="68" priority="15" operator="containsText" text="|">
+    <cfRule type="containsText" dxfId="66" priority="15" operator="containsText" text="|">
       <formula>NOT(ISERROR(SEARCH(("|"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="67" priority="16" operator="containsText" text=")">
+    <cfRule type="containsText" dxfId="65" priority="16" operator="containsText" text=")">
       <formula>NOT(ISERROR(SEARCH((")"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="66" priority="17" operator="containsText" text="(">
+    <cfRule type="containsText" dxfId="64" priority="17" operator="containsText" text="(">
       <formula>NOT(ISERROR(SEARCH(("("),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="65" priority="18" operator="containsText" text="&amp;">
+    <cfRule type="containsText" dxfId="63" priority="18" operator="containsText" text="&amp;">
       <formula>NOT(ISERROR(SEARCH(("&amp;"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="64" priority="19" operator="containsText" text="^">
+    <cfRule type="containsText" dxfId="62" priority="19" operator="containsText" text="^">
       <formula>NOT(ISERROR(SEARCH(("^"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="63" priority="20" operator="containsText" text="%">
+    <cfRule type="containsText" dxfId="61" priority="20" operator="containsText" text="%">
       <formula>NOT(ISERROR(SEARCH(("%"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="62" priority="21" operator="containsText" text="$">
+    <cfRule type="containsText" dxfId="60" priority="21" operator="containsText" text="$">
       <formula>NOT(ISERROR(SEARCH(("$"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="61" priority="22" operator="containsText" text="#">
+    <cfRule type="containsText" dxfId="59" priority="22" operator="containsText" text="#">
       <formula>NOT(ISERROR(SEARCH(("#"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="60" priority="23" operator="containsText" text="@">
+    <cfRule type="containsText" dxfId="58" priority="23" operator="containsText" text="@">
       <formula>NOT(ISERROR(SEARCH(("@"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="59" priority="24" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="57" priority="24" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH(("!"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="58" priority="25" operator="containsText" text="`">
+    <cfRule type="containsText" dxfId="56" priority="25" operator="containsText" text="`">
       <formula>NOT(ISERROR(SEARCH(("`"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1000">
-    <cfRule type="containsText" dxfId="57" priority="26" operator="containsText" text="'">
+    <cfRule type="containsText" dxfId="55" priority="26" operator="containsText" text="'">
       <formula>NOT(ISERROR(SEARCH(("'"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B1000">
-    <cfRule type="expression" dxfId="56" priority="27">
+    <cfRule type="expression" dxfId="54" priority="27">
       <formula>COUNTIF(B:B,B4) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28316,30 +28304,26 @@
       <formula>NOT(ISERROR(SEARCH(("%m"),(G1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I1000">
-    <cfRule type="expression" dxfId="55" priority="54">
-      <formula>COUNTIF(I:I, I4) &gt; 1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G4:G1000">
-    <cfRule type="expression" dxfId="54" priority="55">
+  <conditionalFormatting sqref="G4:I1000">
+    <cfRule type="expression" dxfId="27" priority="54">
       <formula>COUNTIF(G:G, G4) &gt; 1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H1000">
-    <cfRule type="expression" dxfId="27" priority="56">
-      <formula>COUNTIF(H:H, H4) &gt; 1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'description &amp; rules'!$A$3:$A$4</xm:f>
           </x14:formula1>
           <xm:sqref>F4:F1000</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'description &amp; rules'!$A$7:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>E4:E1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -28349,240 +28333,206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="43.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="43.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="43.83203125" style="37"/>
+    <col min="1" max="1" width="43.83203125" style="13"/>
+    <col min="2" max="2" width="57.83203125" style="13" customWidth="1"/>
+    <col min="3" max="16384" width="43.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+    </row>
+    <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>30</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-    </row>
-    <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="27" t="s">
-        <v>31</v>
+      <c r="B3" s="29" t="s">
+        <v>30</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="39"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="27" t="s">
-        <v>32</v>
+      <c r="B4" s="29" t="s">
+        <v>31</v>
       </c>
       <c r="C4" s="38"/>
       <c r="D4" s="39"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-    </row>
-    <row r="6" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+    </row>
+    <row r="7" spans="1:4" ht="32" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+    </row>
+    <row r="8" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+    </row>
+    <row r="10" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+    </row>
+    <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <v>1</v>
+      </c>
+      <c r="B11" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
-        <v>1</v>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+    </row>
+    <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="40"/>
+    </row>
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <v>2</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B13" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
-        <v>2</v>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+    </row>
+    <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+    </row>
+    <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <v>3</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B15" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
-        <v>3</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+    </row>
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="27"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+    </row>
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
         <v>4</v>
       </c>
-      <c r="B13" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
-        <v>5</v>
-      </c>
-      <c r="B15" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <v>6</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>39</v>
+      <c r="B17" s="33" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="38"/>
       <c r="D17" s="39"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
+    </row>
+    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+    </row>
+    <row r="19" spans="1:4" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20">
+        <v>5</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="D19" s="39"/>
+    </row>
+    <row r="20" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+    </row>
+    <row r="21" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
+        <v>6</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B13:D13"/>
+  <mergeCells count="17">
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A18:D18"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="A14:D14"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>